<commit_message>
Test Case end to end for Bank loan with pin
</commit_message>
<xml_diff>
--- a/TestingTool_v2/Robot/ConfigurationFile/Config.xlsx
+++ b/TestingTool_v2/Robot/ConfigurationFile/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_v2\Robot\ConfigurationFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3270F503-4E8E-4CC0-A7EB-4BDCE111638B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82CDEAA-1CBC-41FA-8BE0-C44433DCE455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>C:\GithubPhD\rpa-testing\TestingTool_v2\first.py</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool\Applications\C#Models</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool\Applications\C#Models\SimpleBankLoanCSharp</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>